<commit_message>
Updated TMM file. Steady state calculations work now. Heat transfer coefs seem to high.
</commit_message>
<xml_diff>
--- a/TMM Spacecraftv2.1.xlsx
+++ b/TMM Spacecraftv2.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Thermal interaction" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,6 +14,7 @@
     <sheet name="Nodal plan" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Material" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Heat sources" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="F" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="62">
   <si>
     <t xml:space="preserve">Node vs. Node</t>
   </si>
@@ -436,7 +437,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -469,7 +470,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -543,6 +544,10 @@
     </xf>
     <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -637,7 +642,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.75"/>
@@ -780,7 +785,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1215,13 +1220,13 @@
   </sheetPr>
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1249,30 +1254,31 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="n">
-        <f aca="false">'Conductor plan'!G4</f>
-        <v>136000</v>
+        <v>0</v>
       </c>
       <c r="C2" s="5" t="n">
         <f aca="false">'Conductor plan'!M4</f>
-        <v>1679.012346</v>
+        <v>1679.01234567901</v>
       </c>
       <c r="D2" s="7" t="n">
         <f aca="false">'Conductor plan'!M5</f>
-        <v>3317.073171</v>
+        <v>3317.07317073171</v>
       </c>
       <c r="E2" s="7" t="n">
         <f aca="false">'Conductor plan'!M6</f>
-        <v>35886.33288</v>
+        <v>35886.3328822733</v>
       </c>
       <c r="F2" s="8" t="n">
-        <v>0</v>
+        <f aca="false">1/(1/C2+1/H3+1/H6)</f>
+        <v>63.984092744978</v>
       </c>
       <c r="G2" s="8" t="n">
-        <v>0</v>
+        <f aca="false">1/(1/C2+1/G3)</f>
+        <v>0.679588848746508</v>
       </c>
       <c r="H2" s="7" t="n">
         <f aca="false">'Conductor plan'!M7</f>
-        <v>0.6799983</v>
+        <v>0.67999830000425</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1281,30 +1287,30 @@
       </c>
       <c r="B3" s="5" t="n">
         <f aca="false">C2</f>
-        <v>1679.012346</v>
+        <v>1679.01234567901</v>
       </c>
       <c r="C3" s="7" t="n">
-        <f aca="false">'Conductor plan'!L4</f>
-        <v>1700</v>
+        <v>0</v>
       </c>
       <c r="D3" s="7" t="n">
         <f aca="false">'Conductor plan'!M8</f>
-        <v>1133.333333</v>
+        <v>1133.33333333333</v>
       </c>
       <c r="E3" s="7" t="n">
         <f aca="false">'Conductor plan'!M9</f>
-        <v>1642.71556</v>
+        <v>1642.71555996036</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>0</v>
+        <f aca="false">1/(1/H3+1/F8)</f>
+        <v>66.5190107050572</v>
       </c>
       <c r="G3" s="7" t="n">
         <f aca="false">'Conductor plan'!M11</f>
-        <v>0.6798640272</v>
+        <v>0.679864027194561</v>
       </c>
       <c r="H3" s="7" t="n">
         <f aca="false">'Conductor plan'!M12</f>
-        <v>130.4851557</v>
+        <v>130.485155684287</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1313,27 +1319,30 @@
       </c>
       <c r="B4" s="5" t="n">
         <f aca="false">D2</f>
-        <v>3317.073171</v>
+        <v>3317.07317073171</v>
       </c>
       <c r="C4" s="5" t="n">
         <f aca="false">D3</f>
-        <v>1133.333333</v>
+        <v>1133.33333333333</v>
       </c>
       <c r="D4" s="7" t="n">
-        <f aca="false">'Conductor plan'!L5</f>
-        <v>3400</v>
+        <v>0</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>0</v>
+        <f aca="false">1/(1/C4+1/E3)</f>
+        <v>670.645357070605</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>0</v>
+        <f aca="false">1/(1/D3+1/F3)</f>
+        <v>62.8312412831241</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>0</v>
+        <f aca="false">1/(1/D3+1/G3)</f>
+        <v>0.679456434852118</v>
       </c>
       <c r="H4" s="1" t="n">
-        <v>0</v>
+        <f aca="false">1/(1/D3+1/H3)</f>
+        <v>117.012987012987</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1342,28 +1351,30 @@
       </c>
       <c r="B5" s="5" t="n">
         <f aca="false">E2</f>
-        <v>35886.33288</v>
+        <v>35886.3328822733</v>
       </c>
       <c r="C5" s="5" t="n">
         <f aca="false">E3</f>
-        <v>1642.71556</v>
+        <v>1642.71555996036</v>
       </c>
       <c r="D5" s="5" t="n">
         <f aca="false">E4</f>
-        <v>0</v>
+        <v>670.645357070605</v>
       </c>
       <c r="E5" s="7" t="n">
-        <f aca="false">'Conductor plan'!L6</f>
-        <v>48750</v>
+        <v>0</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>0</v>
+        <f aca="false">1/(1/E3+1/F3)</f>
+        <v>63.9302619978175</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>0</v>
+        <f aca="false">1/(1/E3+1/G3)</f>
+        <v>0.679582771028987</v>
       </c>
       <c r="H5" s="1" t="n">
-        <v>0</v>
+        <f aca="false">1/(1/E3+1/H3)</f>
+        <v>120.88309783278</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1372,30 +1383,30 @@
       </c>
       <c r="B6" s="5" t="n">
         <f aca="false">F2</f>
-        <v>0</v>
+        <v>63.984092744978</v>
       </c>
       <c r="C6" s="5" t="n">
         <f aca="false">F3</f>
-        <v>0</v>
+        <v>66.5190107050572</v>
       </c>
       <c r="D6" s="5" t="n">
         <f aca="false">F4</f>
-        <v>0</v>
+        <v>62.8312412831241</v>
       </c>
       <c r="E6" s="5" t="n">
         <f aca="false">F5</f>
-        <v>0</v>
+        <v>63.9302619978175</v>
       </c>
       <c r="F6" s="7" t="n">
-        <f aca="false">'Conductor plan'!G12</f>
-        <v>1700</v>
+        <v>0</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>0</v>
+        <f aca="false">1/(1/F3+1/G3)</f>
+        <v>0.672985711191282</v>
       </c>
       <c r="H6" s="5" t="n">
         <f aca="false">'Conductor plan'!M13</f>
-        <v>135.6927711</v>
+        <v>135.692771084337</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1404,30 +1415,30 @@
       </c>
       <c r="B7" s="5" t="n">
         <f aca="false">G2</f>
-        <v>0</v>
+        <v>0.679588848746508</v>
       </c>
       <c r="C7" s="5" t="n">
         <f aca="false">G3</f>
-        <v>0.6798640272</v>
+        <v>0.679864027194561</v>
       </c>
       <c r="D7" s="5" t="n">
         <f aca="false">G4</f>
-        <v>0</v>
+        <v>0.679456434852118</v>
       </c>
       <c r="E7" s="5" t="n">
         <f aca="false">G5</f>
-        <v>0</v>
+        <v>0.679582771028987</v>
       </c>
       <c r="F7" s="5" t="n">
         <f aca="false">G6</f>
-        <v>0</v>
+        <v>0.672985711191282</v>
       </c>
       <c r="G7" s="7" t="n">
-        <f aca="false">'Conductor plan'!G7</f>
-        <v>272000</v>
+        <v>0</v>
       </c>
       <c r="H7" s="1" t="n">
-        <v>0</v>
+        <f aca="false">1/(1/G3+1/H3)</f>
+        <v>0.676340106743133</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1436,31 +1447,30 @@
       </c>
       <c r="B8" s="5" t="n">
         <f aca="false">H2</f>
-        <v>0.6799983</v>
+        <v>0.67999830000425</v>
       </c>
       <c r="C8" s="5" t="n">
         <f aca="false">H3</f>
-        <v>130.4851557</v>
+        <v>130.485155684287</v>
       </c>
       <c r="D8" s="5" t="n">
         <f aca="false">H4</f>
-        <v>0</v>
+        <v>117.012987012987</v>
       </c>
       <c r="E8" s="5" t="n">
         <f aca="false">H5</f>
-        <v>0</v>
+        <v>120.88309783278</v>
       </c>
       <c r="F8" s="5" t="n">
         <f aca="false">H6</f>
-        <v>135.6927711</v>
+        <v>135.692771084337</v>
       </c>
       <c r="G8" s="5" t="n">
         <f aca="false">H7</f>
-        <v>0</v>
+        <v>0.676340106743133</v>
       </c>
       <c r="H8" s="7" t="n">
-        <f aca="false">'Conductor plan'!G12</f>
-        <v>1700</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1481,11 +1491,11 @@
   </sheetPr>
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.87"/>
   </cols>
@@ -1716,13 +1726,13 @@
         <v>0.92</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G7" s="1" t="n">
         <v>0</v>
@@ -1731,8 +1741,8 @@
         <v>0</v>
       </c>
       <c r="I7" s="1" t="n">
-        <f aca="false">1371*C7*F7 + 220*C7*G7 + 67.9*B7*H7</f>
-        <v>12613.2</v>
+        <f aca="false">1371*0.9*0.8*C7*F7 + 220*C7*G7 + 67.9*B7*H7</f>
+        <v>4540.752</v>
       </c>
       <c r="J7" s="0" t="n">
         <v>0</v>
@@ -1799,7 +1809,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.88"/>
@@ -1947,7 +1957,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.25"/>
   </cols>
@@ -2015,4 +2025,233 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K20" activeCellId="0" sqref="K20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="27" t="n">
+        <v>0.13695</v>
+      </c>
+      <c r="D2" s="27" t="n">
+        <v>0.092</v>
+      </c>
+      <c r="E2" s="27" t="n">
+        <v>0.1964</v>
+      </c>
+      <c r="F2" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="27" t="n">
+        <v>0.2739</v>
+      </c>
+      <c r="C3" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="27" t="n">
+        <v>0.1603</v>
+      </c>
+      <c r="E3" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="27" t="n">
+        <v>0.4801</v>
+      </c>
+      <c r="G3" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="27" t="n">
+        <v>0.0857</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="27" t="n">
+        <v>0.1213</v>
+      </c>
+      <c r="C4" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="27" t="n">
+        <v>0.3928</v>
+      </c>
+      <c r="C5" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="27" t="n">
+        <v>0.4801</v>
+      </c>
+      <c r="D6" s="27" t="n">
+        <v>0.184</v>
+      </c>
+      <c r="E6" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="27" t="n">
+        <v>0.3359</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="27" t="n">
+        <v>0.5228</v>
+      </c>
+      <c r="D8" s="27" t="n">
+        <v>0.1413</v>
+      </c>
+      <c r="E8" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="27" t="n">
+        <v>0.3359</v>
+      </c>
+      <c r="G8" s="27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the heat transfer coefs of some components
</commit_message>
<xml_diff>
--- a/TMM Spacecraftv2.1.xlsx
+++ b/TMM Spacecraftv2.1.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="70">
   <si>
     <t xml:space="preserve">Node vs. Node</t>
   </si>
@@ -145,7 +145,19 @@
     <t xml:space="preserve">Aplanetary</t>
   </si>
   <si>
-    <t xml:space="preserve">Qexternal</t>
+    <t xml:space="preserve">Qexternal_Earth_sunlight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qexternal_Earth_eclipse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qexternal_Moon_sunlight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qexternal_Moon_eclipse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qexternal_TLI</t>
   </si>
   <si>
     <t xml:space="preserve">Qinternal (generated)</t>
@@ -154,6 +166,21 @@
     <t xml:space="preserve">T0</t>
   </si>
   <si>
+    <t xml:space="preserve">Solar radiation intensity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Earth planetary radiation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Earth albedo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moon albedo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Earth visibility factor</t>
+  </si>
+  <si>
     <t xml:space="preserve">Material</t>
   </si>
   <si>
@@ -227,9 +254,6 @@
   </si>
   <si>
     <t xml:space="preserve">1370 W/m2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solar radiation intensity</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.dropbox.com/s/2e20nnoegw12f4b/Spacecraft_Systems_Engineering_4th_ed_2011.pdf?dl=0</t>
@@ -642,7 +666,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.75"/>
@@ -782,10 +806,10 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="K9" activeCellId="0" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -874,11 +898,11 @@
         <v>1.6</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>0.002</v>
+        <v>0.005</v>
       </c>
       <c r="G4" s="5" t="n">
         <f aca="false">E4*C4/F4</f>
-        <v>136000</v>
+        <v>54400</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>170</v>
@@ -887,15 +911,15 @@
         <v>0.05</v>
       </c>
       <c r="K4" s="1" t="n">
-        <v>0.005</v>
+        <v>0.05</v>
       </c>
       <c r="L4" s="5" t="n">
         <f aca="false">H4*J4/K4</f>
-        <v>1700</v>
+        <v>170</v>
       </c>
       <c r="M4" s="5" t="n">
         <f aca="false">1/(1/G4+1/L4)</f>
-        <v>1679.01234567901</v>
+        <v>169.470404984424</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -912,11 +936,11 @@
         <v>1.6</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>0.002</v>
+        <v>0.005</v>
       </c>
       <c r="G5" s="5" t="n">
         <f aca="false">E5*C5/F5</f>
-        <v>136000</v>
+        <v>54400</v>
       </c>
       <c r="H5" s="1" t="n">
         <v>170</v>
@@ -925,15 +949,15 @@
         <v>0.2</v>
       </c>
       <c r="K5" s="1" t="n">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="L5" s="5" t="n">
         <f aca="false">H5*J5/K5</f>
-        <v>3400</v>
+        <v>340</v>
       </c>
       <c r="M5" s="5" t="n">
         <f aca="false">1/(1/G5+1/L5)</f>
-        <v>3317.07317073171</v>
+        <v>337.888198757764</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -950,11 +974,11 @@
         <v>1.6</v>
       </c>
       <c r="F6" s="1" t="n">
-        <v>0.002</v>
+        <v>0.005</v>
       </c>
       <c r="G6" s="5" t="n">
         <f aca="false">E6*C6/F6</f>
-        <v>136000</v>
+        <v>54400</v>
       </c>
       <c r="H6" s="1" t="n">
         <v>97.5</v>
@@ -963,54 +987,29 @@
         <v>1</v>
       </c>
       <c r="K6" s="1" t="n">
-        <v>0.002</v>
+        <v>0.5</v>
       </c>
       <c r="L6" s="5" t="n">
         <f aca="false">H6*J6/K6</f>
-        <v>48750</v>
+        <v>195</v>
       </c>
       <c r="M6" s="5" t="n">
         <f aca="false">1/(1/G6+1/L6)</f>
-        <v>35886.3328822733</v>
+        <v>194.30350764722</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>170</v>
-      </c>
-      <c r="E7" s="1" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="F7" s="1" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="G7" s="5" t="n">
-        <f aca="false">E7*C7/F7</f>
-        <v>272000</v>
-      </c>
-      <c r="H7" s="1" t="n">
-        <v>170</v>
-      </c>
-      <c r="J7" s="1" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="K7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="L7" s="5" t="n">
-        <f aca="false">H7*J7/K7</f>
-        <v>0.68</v>
-      </c>
-      <c r="M7" s="5" t="n">
-        <f aca="false">1/(1/G7+1/L7)</f>
-        <v>0.67999830000425</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
@@ -1026,11 +1025,11 @@
         <v>0.05</v>
       </c>
       <c r="F8" s="1" t="n">
-        <v>0.005</v>
+        <v>0.05</v>
       </c>
       <c r="G8" s="5" t="n">
         <f aca="false">E8*C8/F8</f>
-        <v>1700</v>
+        <v>170</v>
       </c>
       <c r="H8" s="1" t="n">
         <v>170</v>
@@ -1039,15 +1038,15 @@
         <v>0.2</v>
       </c>
       <c r="K8" s="1" t="n">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="L8" s="5" t="n">
         <f aca="false">H8*J8/K8</f>
-        <v>3400</v>
+        <v>340</v>
       </c>
       <c r="M8" s="5" t="n">
         <f aca="false">1/(1/G8+1/L8)</f>
-        <v>1133.33333333333</v>
+        <v>113.333333333333</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1064,11 +1063,11 @@
         <v>0.05</v>
       </c>
       <c r="F9" s="1" t="n">
-        <v>0.005</v>
+        <v>0.05</v>
       </c>
       <c r="G9" s="5" t="n">
         <f aca="false">E9*C9/F9</f>
-        <v>1700</v>
+        <v>170</v>
       </c>
       <c r="H9" s="6" t="n">
         <v>97.5</v>
@@ -1077,18 +1076,18 @@
         <v>1</v>
       </c>
       <c r="K9" s="1" t="n">
-        <v>0.002</v>
+        <v>0.5</v>
       </c>
       <c r="L9" s="5" t="n">
         <f aca="false">H9*J9/K9</f>
-        <v>48750</v>
+        <v>195</v>
       </c>
       <c r="M9" s="5" t="n">
         <f aca="false">1/(1/G9+1/L9)</f>
-        <v>1642.71555996036</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>90.8219178082192</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -1102,28 +1101,28 @@
         <v>0.1</v>
       </c>
       <c r="F11" s="1" t="n">
-        <v>0.005</v>
+        <v>0.05</v>
       </c>
       <c r="G11" s="5" t="n">
         <f aca="false">E11*C11/F11</f>
-        <v>3400</v>
+        <v>340</v>
       </c>
       <c r="H11" s="1" t="n">
         <v>170</v>
       </c>
       <c r="J11" s="1" t="n">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="K11" s="1" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L11" s="5" t="n">
         <f aca="false">H11*J11/K11</f>
-        <v>0.68</v>
+        <v>8.5</v>
       </c>
       <c r="M11" s="5" t="n">
         <f aca="false">1/(1/G11+1/L11)</f>
-        <v>0.679864027194561</v>
+        <v>8.29268292682927</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1140,11 +1139,11 @@
         <v>0.05</v>
       </c>
       <c r="F12" s="1" t="n">
-        <v>0.005</v>
+        <v>0.05</v>
       </c>
       <c r="G12" s="5" t="n">
         <f aca="false">E12*C12/F12</f>
-        <v>1700</v>
+        <v>170</v>
       </c>
       <c r="H12" s="6" t="n">
         <v>0.53</v>
@@ -1153,15 +1152,15 @@
         <v>0.8</v>
       </c>
       <c r="K12" s="1" t="n">
-        <v>0.003</v>
+        <v>0.002</v>
       </c>
       <c r="L12" s="5" t="n">
         <f aca="false">H12*J12/K12</f>
-        <v>141.333333333333</v>
+        <v>212</v>
       </c>
       <c r="M12" s="5" t="n">
         <f aca="false">1/(1/G12+1/L12)</f>
-        <v>130.485155684287</v>
+        <v>94.3455497382199</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1191,15 +1190,15 @@
         <v>0.8</v>
       </c>
       <c r="K13" s="1" t="n">
-        <v>0.003</v>
+        <v>0.002</v>
       </c>
       <c r="L13" s="5" t="n">
         <f aca="false">H13*J13/K13</f>
-        <v>141.333333333333</v>
+        <v>212</v>
       </c>
       <c r="M13" s="5" t="n">
         <f aca="false">1/(1/G13+1/L13)</f>
-        <v>135.692771084337</v>
+        <v>199.557032115172</v>
       </c>
     </row>
   </sheetData>
@@ -1221,10 +1220,10 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -1258,27 +1257,27 @@
       </c>
       <c r="C2" s="5" t="n">
         <f aca="false">'Conductor plan'!M4</f>
-        <v>1679.01234567901</v>
+        <v>169.470404984424</v>
       </c>
       <c r="D2" s="7" t="n">
         <f aca="false">'Conductor plan'!M5</f>
-        <v>3317.07317073171</v>
+        <v>337.888198757764</v>
       </c>
       <c r="E2" s="7" t="n">
         <f aca="false">'Conductor plan'!M6</f>
-        <v>35886.3328822733</v>
+        <v>194.30350764722</v>
       </c>
       <c r="F2" s="8" t="n">
         <f aca="false">1/(1/C2+1/H3+1/H6)</f>
-        <v>63.984092744978</v>
+        <v>46.4874800470808</v>
       </c>
       <c r="G2" s="8" t="n">
         <f aca="false">1/(1/C2+1/G3)</f>
-        <v>0.679588848746508</v>
+        <v>7.9058276413312</v>
       </c>
       <c r="H2" s="7" t="n">
         <f aca="false">'Conductor plan'!M7</f>
-        <v>0.67999830000425</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1287,30 +1286,30 @@
       </c>
       <c r="B3" s="5" t="n">
         <f aca="false">C2</f>
-        <v>1679.01234567901</v>
+        <v>169.470404984424</v>
       </c>
       <c r="C3" s="7" t="n">
         <v>0</v>
       </c>
       <c r="D3" s="7" t="n">
         <f aca="false">'Conductor plan'!M8</f>
-        <v>1133.33333333333</v>
+        <v>113.333333333333</v>
       </c>
       <c r="E3" s="7" t="n">
         <f aca="false">'Conductor plan'!M9</f>
-        <v>1642.71555996036</v>
+        <v>90.8219178082192</v>
       </c>
       <c r="F3" s="1" t="n">
         <f aca="false">1/(1/H3+1/F8)</f>
-        <v>66.5190107050572</v>
+        <v>64.0597227159616</v>
       </c>
       <c r="G3" s="7" t="n">
         <f aca="false">'Conductor plan'!M11</f>
-        <v>0.679864027194561</v>
+        <v>8.29268292682927</v>
       </c>
       <c r="H3" s="7" t="n">
         <f aca="false">'Conductor plan'!M12</f>
-        <v>130.485155684287</v>
+        <v>94.3455497382199</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1319,30 +1318,30 @@
       </c>
       <c r="B4" s="5" t="n">
         <f aca="false">D2</f>
-        <v>3317.07317073171</v>
+        <v>337.888198757764</v>
       </c>
       <c r="C4" s="5" t="n">
         <f aca="false">D3</f>
-        <v>1133.33333333333</v>
+        <v>113.333333333333</v>
       </c>
       <c r="D4" s="7" t="n">
         <v>0</v>
       </c>
       <c r="E4" s="1" t="n">
         <f aca="false">1/(1/C4+1/E3)</f>
-        <v>670.645357070605</v>
+        <v>50.4182509505703</v>
       </c>
       <c r="F4" s="1" t="n">
         <f aca="false">1/(1/D3+1/F3)</f>
-        <v>62.8312412831241</v>
+        <v>40.9266409266409</v>
       </c>
       <c r="G4" s="1" t="n">
         <f aca="false">1/(1/D3+1/G3)</f>
-        <v>0.679456434852118</v>
+        <v>7.72727272727273</v>
       </c>
       <c r="H4" s="1" t="n">
         <f aca="false">1/(1/D3+1/H3)</f>
-        <v>117.012987012987</v>
+        <v>51.4857142857143</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1351,30 +1350,30 @@
       </c>
       <c r="B5" s="5" t="n">
         <f aca="false">E2</f>
-        <v>35886.3328822733</v>
+        <v>194.30350764722</v>
       </c>
       <c r="C5" s="5" t="n">
         <f aca="false">E3</f>
-        <v>1642.71555996036</v>
+        <v>90.8219178082192</v>
       </c>
       <c r="D5" s="5" t="n">
         <f aca="false">E4</f>
-        <v>670.645357070605</v>
+        <v>50.4182509505703</v>
       </c>
       <c r="E5" s="7" t="n">
         <v>0</v>
       </c>
       <c r="F5" s="1" t="n">
         <f aca="false">1/(1/E3+1/F3)</f>
-        <v>63.9302619978175</v>
+        <v>37.5643417233693</v>
       </c>
       <c r="G5" s="1" t="n">
         <f aca="false">1/(1/E3+1/G3)</f>
-        <v>0.679582771028987</v>
+        <v>7.59885386819484</v>
       </c>
       <c r="H5" s="1" t="n">
         <f aca="false">1/(1/E3+1/H3)</f>
-        <v>120.88309783278</v>
+        <v>46.2751037071179</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1383,30 +1382,30 @@
       </c>
       <c r="B6" s="5" t="n">
         <f aca="false">F2</f>
-        <v>63.984092744978</v>
+        <v>46.4874800470808</v>
       </c>
       <c r="C6" s="5" t="n">
         <f aca="false">F3</f>
-        <v>66.5190107050572</v>
+        <v>64.0597227159616</v>
       </c>
       <c r="D6" s="5" t="n">
         <f aca="false">F4</f>
-        <v>62.8312412831241</v>
+        <v>40.9266409266409</v>
       </c>
       <c r="E6" s="5" t="n">
         <f aca="false">F5</f>
-        <v>63.9302619978175</v>
+        <v>37.5643417233693</v>
       </c>
       <c r="F6" s="7" t="n">
         <v>0</v>
       </c>
       <c r="G6" s="1" t="n">
         <f aca="false">1/(1/F3+1/G3)</f>
-        <v>0.672985711191282</v>
+        <v>7.34221570305179</v>
       </c>
       <c r="H6" s="5" t="n">
         <f aca="false">'Conductor plan'!M13</f>
-        <v>135.692771084337</v>
+        <v>199.557032115172</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1415,30 +1414,30 @@
       </c>
       <c r="B7" s="5" t="n">
         <f aca="false">G2</f>
-        <v>0.679588848746508</v>
+        <v>7.9058276413312</v>
       </c>
       <c r="C7" s="5" t="n">
         <f aca="false">G3</f>
-        <v>0.679864027194561</v>
+        <v>8.29268292682927</v>
       </c>
       <c r="D7" s="5" t="n">
         <f aca="false">G4</f>
-        <v>0.679456434852118</v>
+        <v>7.72727272727273</v>
       </c>
       <c r="E7" s="5" t="n">
         <f aca="false">G5</f>
-        <v>0.679582771028987</v>
+        <v>7.59885386819484</v>
       </c>
       <c r="F7" s="5" t="n">
         <f aca="false">G6</f>
-        <v>0.672985711191282</v>
+        <v>7.34221570305179</v>
       </c>
       <c r="G7" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H7" s="1" t="n">
         <f aca="false">1/(1/G3+1/H3)</f>
-        <v>0.676340106743133</v>
+        <v>7.62267343485618</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1447,27 +1446,27 @@
       </c>
       <c r="B8" s="5" t="n">
         <f aca="false">H2</f>
-        <v>0.67999830000425</v>
+        <v>0</v>
       </c>
       <c r="C8" s="5" t="n">
         <f aca="false">H3</f>
-        <v>130.485155684287</v>
+        <v>94.3455497382199</v>
       </c>
       <c r="D8" s="5" t="n">
         <f aca="false">H4</f>
-        <v>117.012987012987</v>
+        <v>51.4857142857143</v>
       </c>
       <c r="E8" s="5" t="n">
         <f aca="false">H5</f>
-        <v>120.88309783278</v>
+        <v>46.2751037071179</v>
       </c>
       <c r="F8" s="5" t="n">
         <f aca="false">H6</f>
-        <v>135.692771084337</v>
+        <v>199.557032115172</v>
       </c>
       <c r="G8" s="5" t="n">
         <f aca="false">H7</f>
-        <v>0.676340106743133</v>
+        <v>7.62267343485618</v>
       </c>
       <c r="H8" s="7" t="n">
         <v>0</v>
@@ -1489,18 +1488,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="10" style="0" width="16.87"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1534,16 +1533,43 @@
       <c r="K1" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="T1" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="n">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="C2" s="6" t="n">
-        <v>0.15</v>
+        <v>0.25</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>9.6</v>
@@ -1561,14 +1587,45 @@
         <v>1.6</v>
       </c>
       <c r="I2" s="1" t="n">
-        <f aca="false">1371*C2*F2 + 220*C2*G2 + 67.9*B2*H2</f>
-        <v>387.272</v>
+        <f aca="false">P2*C2*F2 + Q2*C2*H2 + P2*R2*T2*B2*G2</f>
+        <v>663.5458</v>
       </c>
       <c r="J2" s="1" t="n">
-        <v>0</v>
+        <f aca="false">Q2*C2*G2 + P2*R2*T2*B2*H2</f>
+        <v>115.1458</v>
       </c>
       <c r="K2" s="1" t="n">
+        <f aca="false">P2*F2*C2+P2*G2*C2*T2*S2</f>
+        <v>558.2712</v>
+      </c>
+      <c r="L2" s="1" t="n">
+        <f aca="false">P2*G2*C2*T2*S2</f>
+        <v>9.8712</v>
+      </c>
+      <c r="M2" s="1" t="n">
+        <f aca="false">P2*F2*C2</f>
+        <v>548.4</v>
+      </c>
+      <c r="N2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1" t="n">
         <v>273</v>
+      </c>
+      <c r="P2" s="0" t="n">
+        <v>1371</v>
+      </c>
+      <c r="Q2" s="0" t="n">
+        <v>220</v>
+      </c>
+      <c r="R2" s="0" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="S2" s="0" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="T2" s="0" t="n">
+        <v>0.15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1597,14 +1654,45 @@
         <v>0</v>
       </c>
       <c r="I3" s="1" t="n">
-        <f aca="false">1371*C3*F3 + 220*C3*G3 + 67.9*B3*H3</f>
+        <f aca="false">P3*C3*F3 + Q3*C3*H3 + P3*R3*T3*B3*G3</f>
         <v>0</v>
       </c>
       <c r="J3" s="1" t="n">
+        <f aca="false">Q3*C3*G3 + P3*R3*T3*B3*H3</f>
         <v>0</v>
       </c>
       <c r="K3" s="1" t="n">
+        <f aca="false">P3*F3*C3+P3*G3*C3*T3*S3</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="1" t="n">
+        <f aca="false">P3*G3*C3*T3*S3</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="1" t="n">
+        <f aca="false">P3*F3*C3</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" s="1" t="n">
         <v>273</v>
+      </c>
+      <c r="P3" s="0" t="n">
+        <v>1371</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <v>220</v>
+      </c>
+      <c r="R3" s="0" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="S3" s="0" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="T3" s="0" t="n">
+        <v>0.15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1612,10 +1700,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="9" t="n">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="C4" s="9" t="n">
-        <v>0.5</v>
+        <v>0.14</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>0.6</v>
@@ -1633,14 +1721,45 @@
         <v>0.1</v>
       </c>
       <c r="I4" s="1" t="n">
-        <f aca="false">1371*C4*F4 + 220*C4*G4 + 67.9*B4*H4</f>
-        <v>82.945</v>
+        <f aca="false">P4*C4*F4 + Q4*C4*H4 + P4*R4*T4*B4*G4</f>
+        <v>22.6133225</v>
       </c>
       <c r="J4" s="1" t="n">
+        <f aca="false">Q4*C4*G4 + P4*R4*T4*B4*H4</f>
+        <v>3.4193225</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <f aca="false">P4*F4*C4+P4*G4*C4*T4*S4</f>
+        <v>19.539492</v>
+      </c>
+      <c r="L4" s="1" t="n">
+        <f aca="false">P4*G4*C4*T4*S4</f>
+        <v>0.345492</v>
+      </c>
+      <c r="M4" s="1" t="n">
+        <f aca="false">P4*F4*C4</f>
+        <v>19.194</v>
+      </c>
+      <c r="N4" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="K4" s="1" t="n">
+      <c r="O4" s="1" t="n">
         <v>273</v>
+      </c>
+      <c r="P4" s="0" t="n">
+        <v>1371</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <v>220</v>
+      </c>
+      <c r="R4" s="0" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="S4" s="0" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="T4" s="0" t="n">
+        <v>0.15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1669,14 +1788,45 @@
         <v>0.7</v>
       </c>
       <c r="I5" s="1" t="n">
-        <f aca="false">1371*C5*F5 + 220*C5*G5 + 67.9*B5*H5</f>
-        <v>765.42</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <v>0</v>
+        <f aca="false">P5*C5*F5 + Q5*C5*H5 + P5*R5*T5*B5*G5</f>
+        <v>784.4618</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <f aca="false">Q5*C5*G5 + P5*R5*T5*B5*H5</f>
+        <v>112.80412</v>
       </c>
       <c r="K5" s="1" t="n">
+        <f aca="false">P5*F5*C5+P5*G5*C5*T5*S5</f>
+        <v>660.98652</v>
+      </c>
+      <c r="L5" s="1" t="n">
+        <f aca="false">P5*G5*C5*T5*S5</f>
+        <v>8.39052</v>
+      </c>
+      <c r="M5" s="1" t="n">
+        <f aca="false">P5*F5*C5</f>
+        <v>652.596</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1" t="n">
         <v>273</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <v>1371</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <v>220</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="S5" s="0" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="T5" s="0" t="n">
+        <v>0.15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1705,14 +1855,45 @@
         <v>0</v>
       </c>
       <c r="I6" s="1" t="n">
-        <f aca="false">1371*C6*F6 + 220*C6*G6 + 67.9*B6*H6</f>
+        <f aca="false">P6*C6*F6 + Q6*C6*H6 + P6*R6*T6*B6*G6</f>
         <v>0</v>
       </c>
       <c r="J6" s="1" t="n">
+        <f aca="false">Q6*C6*G6 + P6*R6*T6*B6*H6</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <f aca="false">P6*F6*C6+P6*G6*C6*T6*S6</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="1" t="n">
+        <f aca="false">P6*G6*C6*T6*S6</f>
+        <v>0</v>
+      </c>
+      <c r="M6" s="1" t="n">
+        <f aca="false">P6*F6*C6</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="K6" s="1" t="n">
+      <c r="O6" s="1" t="n">
         <v>273</v>
+      </c>
+      <c r="P6" s="0" t="n">
+        <v>1371</v>
+      </c>
+      <c r="Q6" s="0" t="n">
+        <v>220</v>
+      </c>
+      <c r="R6" s="0" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="S6" s="0" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="T6" s="0" t="n">
+        <v>0.15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1741,14 +1922,45 @@
         <v>0</v>
       </c>
       <c r="I7" s="1" t="n">
-        <f aca="false">1371*0.9*0.8*C7*F7 + 220*C7*G7 + 67.9*B7*H7</f>
-        <v>4540.752</v>
-      </c>
-      <c r="J7" s="0" t="n">
+        <f aca="false">P7*C7*F7 + Q7*C7*H7 + P7*R7*T7*B7*G7</f>
+        <v>6306.6</v>
+      </c>
+      <c r="J7" s="1" t="n">
+        <f aca="false">Q7*C7*G7 + P7*R7*T7*B7*H7</f>
         <v>0</v>
       </c>
       <c r="K7" s="1" t="n">
+        <f aca="false">P7*F7*C7+P7*G7*C7*T7*S7</f>
+        <v>6306.6</v>
+      </c>
+      <c r="L7" s="1" t="n">
+        <f aca="false">P7*G7*C7*T7*S7</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="1" t="n">
+        <f aca="false">P7*F7*C7</f>
+        <v>6306.6</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" s="1" t="n">
         <v>273</v>
+      </c>
+      <c r="P7" s="0" t="n">
+        <v>1371</v>
+      </c>
+      <c r="Q7" s="0" t="n">
+        <v>220</v>
+      </c>
+      <c r="R7" s="0" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="S7" s="0" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="T7" s="0" t="n">
+        <v>0.15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1776,14 +1988,46 @@
       <c r="H8" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" s="0" t="n">
+      <c r="I8" s="1" t="n">
+        <f aca="false">P8*C8*F8 + Q8*C8*H8 + P8*R8*T8*B8*G8</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="1" t="n">
+        <f aca="false">Q8*C8*G8 + P8*R8*T8*B8*H8</f>
         <v>0</v>
       </c>
       <c r="K8" s="1" t="n">
+        <f aca="false">P8*F8*C8+P8*G8*C8*T8*S8</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="1" t="n">
+        <f aca="false">P8*G8*C8*T8*S8</f>
+        <v>0</v>
+      </c>
+      <c r="M8" s="1" t="n">
+        <f aca="false">P8*F8*C8</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" s="1" t="n">
         <v>273</v>
+      </c>
+      <c r="P8" s="0" t="n">
+        <v>1371</v>
+      </c>
+      <c r="Q8" s="0" t="n">
+        <v>220</v>
+      </c>
+      <c r="R8" s="0" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="S8" s="0" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="T8" s="0" t="n">
+        <v>0.15</v>
       </c>
     </row>
   </sheetData>
@@ -1806,10 +2050,10 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.88"/>
@@ -1818,28 +2062,28 @@
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11"/>
       <c r="B1" s="12" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>12</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
@@ -1850,10 +2094,10 @@
       <c r="A2" s="15"/>
       <c r="B2" s="16"/>
       <c r="C2" s="17" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>16</v>
@@ -1869,7 +2113,7 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="18" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C3" s="19" t="n">
         <v>896</v>
@@ -1882,44 +2126,44 @@
       </c>
       <c r="F3" s="21"/>
       <c r="G3" s="22" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="18" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
       <c r="F4" s="21" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="G4" s="22" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="H4" s="22" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1927,7 +2171,7 @@
         <v>7</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1957,28 +2201,28 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.25"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="24" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1986,10 +2230,10 @@
         <v>0.9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2038,7 +2282,7 @@
       <selection pane="topLeft" activeCell="K20" activeCellId="0" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">

</xml_diff>